<commit_message>
Update xlsx for google mymap
</commit_message>
<xml_diff>
--- a/us-states.xlsx
+++ b/us-states.xlsx
@@ -12,24 +12,25 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312"/>
   </bookViews>
   <sheets>
-    <sheet name="States" sheetId="1" r:id="rId1"/>
-    <sheet name="us-states" sheetId="2" r:id="rId2"/>
+    <sheet name="ForGoogleMap" sheetId="3" r:id="rId1"/>
+    <sheet name="States" sheetId="1" r:id="rId2"/>
+    <sheet name="us-states" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_FC6203C8_E714_4EFF_8F5E_C643AB73B894_.wvu.FilterData" localSheetId="0" hidden="1">States!$A$1:$Y$58</definedName>
+    <definedName name="Z_FC6203C8_E714_4EFF_8F5E_C643AB73B894_.wvu.FilterData" localSheetId="1" hidden="1">States!$A$1:$Y$58</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{FC6203C8-E714-4EFF-8F5E-C643AB73B894}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3218" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3274" uniqueCount="65">
   <si>
     <t>date</t>
   </si>
@@ -223,15 +224,17 @@
     <t>總計</t>
   </si>
   <si>
-    <t>DeathRate</t>
+    <t>DeathRate(%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.0000000_);_(* \(#,##0.0000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -343,9 +346,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -370,9 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -380,9 +380,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -394,15 +391,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="千分位" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
@@ -435,7 +459,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Wei-Shun Lo" refreshedDate="43951.171034375002" refreshedVersion="5" recordCount="1501">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Wei-Shun Lo" refreshedDate="43951.183772453704" refreshedVersion="5" recordCount="1501">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1502" sheet="us-states"/>
   </cacheSource>
@@ -11034,7 +11058,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="States" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="States" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
   <location ref="A1:C58" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField name="date" compact="0" numFmtId="164" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
@@ -11292,13 +11316,13 @@
     <dataField name="SUM of deaths" fld="4" baseField="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="5">
+    <format dxfId="11">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="10">
       <pivotArea outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="50">
@@ -11356,7 +11380,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="5">
@@ -11369,10 +11393,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -11650,33 +11674,906 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41:G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.88671875" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="8">
+        <v>5130</v>
+      </c>
+      <c r="C2" s="9">
+        <v>28</v>
+      </c>
+      <c r="D2" s="16">
+        <f>C2/B2*100</f>
+        <v>0.54580896686159852</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="11">
+        <v>717</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17">
+        <f t="shared" ref="D3:D57" si="0">C3/B3*100</f>
+        <v>0.69735006973500702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11">
+        <v>4397</v>
+      </c>
+      <c r="C4" s="12">
+        <v>74</v>
+      </c>
+      <c r="D4" s="17">
+        <f t="shared" si="0"/>
+        <v>1.6829656584034569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2897</v>
+      </c>
+      <c r="C5" s="12">
+        <v>21</v>
+      </c>
+      <c r="D5" s="17">
+        <f t="shared" si="0"/>
+        <v>0.72488781498101484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11">
+        <v>39644</v>
+      </c>
+      <c r="C6" s="12">
+        <v>775</v>
+      </c>
+      <c r="D6" s="17">
+        <f t="shared" si="0"/>
+        <v>1.9548985975179094</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="11">
+        <v>12985</v>
+      </c>
+      <c r="C7" s="12">
+        <v>224</v>
+      </c>
+      <c r="D7" s="17">
+        <f t="shared" si="0"/>
+        <v>1.725067385444744</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="11">
+        <v>8907</v>
+      </c>
+      <c r="C8" s="12">
+        <v>178</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" si="0"/>
+        <v>1.9984282025373303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1304</v>
+      </c>
+      <c r="C9" s="12">
+        <v>14</v>
+      </c>
+      <c r="D9" s="17">
+        <f t="shared" si="0"/>
+        <v>1.0736196319018405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2027</v>
+      </c>
+      <c r="C10" s="12">
+        <v>23</v>
+      </c>
+      <c r="D10" s="17">
+        <f t="shared" si="0"/>
+        <v>1.1346817957572768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="11">
+        <v>23152</v>
+      </c>
+      <c r="C11" s="12">
+        <v>330</v>
+      </c>
+      <c r="D11" s="17">
+        <f t="shared" si="0"/>
+        <v>1.4253628196268142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="11">
+        <v>14977</v>
+      </c>
+      <c r="C12" s="12">
+        <v>470</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" si="0"/>
+        <v>3.1381451559057223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="11">
+        <v>395</v>
+      </c>
+      <c r="C13" s="12">
+        <v>8</v>
+      </c>
+      <c r="D13" s="17">
+        <f t="shared" si="0"/>
+        <v>2.0253164556962027</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1046</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1416</v>
+      </c>
+      <c r="C15" s="12">
+        <v>18</v>
+      </c>
+      <c r="D15" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2711864406779663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="11">
+        <v>22173</v>
+      </c>
+      <c r="C16" s="12">
+        <v>258</v>
+      </c>
+      <c r="D16" s="17">
+        <f t="shared" si="0"/>
+        <v>1.1635773237721554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="11">
+        <v>6126</v>
+      </c>
+      <c r="C17" s="12">
+        <v>160</v>
+      </c>
+      <c r="D17" s="17">
+        <f t="shared" si="0"/>
+        <v>2.6118184786157359</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1869</v>
+      </c>
+      <c r="C18" s="12">
+        <v>13</v>
+      </c>
+      <c r="D18" s="17">
+        <f t="shared" si="0"/>
+        <v>0.69555912252541463</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1589</v>
+      </c>
+      <c r="C19" s="12">
+        <v>41</v>
+      </c>
+      <c r="D19" s="17">
+        <f t="shared" si="0"/>
+        <v>2.5802391441157964</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2328</v>
+      </c>
+      <c r="C20" s="12">
+        <v>55</v>
+      </c>
+      <c r="D20" s="17">
+        <f t="shared" si="0"/>
+        <v>2.3625429553264605</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="11">
+        <v>19653</v>
+      </c>
+      <c r="C21" s="12">
+        <v>710</v>
+      </c>
+      <c r="D21" s="17">
+        <f t="shared" si="0"/>
+        <v>3.6126799979646873</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1532</v>
+      </c>
+      <c r="C22" s="12">
+        <v>5</v>
+      </c>
+      <c r="D22" s="17">
+        <f t="shared" si="0"/>
+        <v>0.32637075718015662</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="11">
+        <v>5739</v>
+      </c>
+      <c r="C23" s="12">
+        <v>51</v>
+      </c>
+      <c r="D23" s="17">
+        <f t="shared" si="0"/>
+        <v>0.8886565603763722</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="11">
+        <v>22075</v>
+      </c>
+      <c r="C24" s="12">
+        <v>195</v>
+      </c>
+      <c r="D24" s="17">
+        <f t="shared" si="0"/>
+        <v>0.88335220838052098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="11">
+        <v>25093</v>
+      </c>
+      <c r="C25" s="12">
+        <v>505</v>
+      </c>
+      <c r="D25" s="17">
+        <f t="shared" si="0"/>
+        <v>2.0125134499661259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="11">
+        <v>3270</v>
+      </c>
+      <c r="C26" s="12">
+        <v>25</v>
+      </c>
+      <c r="D26" s="17">
+        <f t="shared" si="0"/>
+        <v>0.76452599388379205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="11">
+        <v>4008</v>
+      </c>
+      <c r="C27" s="12">
+        <v>52</v>
+      </c>
+      <c r="D27" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2974051896207583</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="11">
+        <v>4132</v>
+      </c>
+      <c r="C28" s="12">
+        <v>67</v>
+      </c>
+      <c r="D28" s="17">
+        <f t="shared" si="0"/>
+        <v>1.6214908034849953</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="11">
+        <v>825</v>
+      </c>
+      <c r="C29" s="12">
+        <v>3</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="11">
+        <v>1447</v>
+      </c>
+      <c r="C30" s="12">
+        <v>6</v>
+      </c>
+      <c r="D30" s="17">
+        <f t="shared" si="0"/>
+        <v>0.414651002073255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="11">
+        <v>4702</v>
+      </c>
+      <c r="C31" s="12">
+        <v>79</v>
+      </c>
+      <c r="D31" s="17">
+        <f t="shared" si="0"/>
+        <v>1.6801361122926413</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="11">
+        <v>1551</v>
+      </c>
+      <c r="C32" s="12">
+        <v>11</v>
+      </c>
+      <c r="D32" s="17">
+        <f t="shared" si="0"/>
+        <v>0.70921985815602839</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="11">
+        <v>57202</v>
+      </c>
+      <c r="C33" s="12">
+        <v>698</v>
+      </c>
+      <c r="D33" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2202370546484387</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="11">
+        <v>1389</v>
+      </c>
+      <c r="C34" s="12">
+        <v>7</v>
+      </c>
+      <c r="D34" s="17">
+        <f t="shared" si="0"/>
+        <v>0.5039596832253419</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="11">
+        <v>320540</v>
+      </c>
+      <c r="C35" s="12">
+        <v>3767</v>
+      </c>
+      <c r="D35" s="17">
+        <f t="shared" si="0"/>
+        <v>1.1752043426717416</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="11">
+        <v>5790</v>
+      </c>
+      <c r="C36" s="12">
+        <v>16</v>
+      </c>
+      <c r="D36" s="17">
+        <f t="shared" si="0"/>
+        <v>0.27633851468048359</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="11">
+        <v>553</v>
+      </c>
+      <c r="C37" s="12">
+        <v>3</v>
+      </c>
+      <c r="D37" s="17">
+        <f t="shared" si="0"/>
+        <v>0.54249547920433994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="11">
+        <v>4</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+      <c r="D38" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="11">
+        <v>7981</v>
+      </c>
+      <c r="C39" s="12">
+        <v>124</v>
+      </c>
+      <c r="D39" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5536900137827339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="11">
+        <v>2022</v>
+      </c>
+      <c r="C40" s="12">
+        <v>61</v>
+      </c>
+      <c r="D40" s="17">
+        <f t="shared" si="0"/>
+        <v>3.0168150346191891</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="11">
+        <v>3323</v>
+      </c>
+      <c r="C41" s="12">
+        <v>95</v>
+      </c>
+      <c r="D41" s="17">
+        <f t="shared" si="0"/>
+        <v>2.8588624736683723</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="11">
+        <v>14707</v>
+      </c>
+      <c r="C42" s="12">
+        <v>146</v>
+      </c>
+      <c r="D42" s="17">
+        <f t="shared" si="0"/>
+        <v>0.99272455293397699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="11">
+        <v>582</v>
+      </c>
+      <c r="C43" s="12">
+        <v>21</v>
+      </c>
+      <c r="D43" s="17">
+        <f t="shared" si="0"/>
+        <v>3.608247422680412</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="11">
+        <v>1674</v>
+      </c>
+      <c r="C44" s="12">
+        <v>5</v>
+      </c>
+      <c r="D44" s="17">
+        <f t="shared" si="0"/>
+        <v>0.29868578255675032</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="11">
+        <v>4315</v>
+      </c>
+      <c r="C45" s="12">
+        <v>85</v>
+      </c>
+      <c r="D45" s="17">
+        <f t="shared" si="0"/>
+        <v>1.9698725376593278</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="11">
+        <v>504</v>
+      </c>
+      <c r="C46" s="12">
+        <v>20</v>
+      </c>
+      <c r="D46" s="17">
+        <f t="shared" si="0"/>
+        <v>3.9682539682539679</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="11">
+        <v>8593</v>
+      </c>
+      <c r="C47" s="12">
+        <v>33</v>
+      </c>
+      <c r="D47" s="17">
+        <f t="shared" si="0"/>
+        <v>0.38403351565227511</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="11">
+        <v>13774</v>
+      </c>
+      <c r="C48" s="12">
+        <v>163</v>
+      </c>
+      <c r="D48" s="17">
+        <f t="shared" si="0"/>
+        <v>1.1833889937563524</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="11">
+        <v>3873</v>
+      </c>
+      <c r="C49" s="12">
+        <v>11</v>
+      </c>
+      <c r="D49" s="17">
+        <f t="shared" si="0"/>
+        <v>0.28401755744900598</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="11">
+        <v>1301</v>
+      </c>
+      <c r="C50" s="12">
+        <v>68</v>
+      </c>
+      <c r="D50" s="17">
+        <f t="shared" si="0"/>
+        <v>5.2267486548808613</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="11">
+        <v>170</v>
+      </c>
+      <c r="C51" s="12">
+        <v>0</v>
+      </c>
+      <c r="D51" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="11">
+        <v>4711</v>
+      </c>
+      <c r="C52" s="12">
+        <v>109</v>
+      </c>
+      <c r="D52" s="17">
+        <f t="shared" si="0"/>
+        <v>2.3137338144767567</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="11">
+        <v>35811</v>
+      </c>
+      <c r="C53" s="12">
+        <v>1924</v>
+      </c>
+      <c r="D53" s="17">
+        <f t="shared" si="0"/>
+        <v>5.3726508614671475</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="11">
+        <v>559</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1</v>
+      </c>
+      <c r="D54" s="17">
+        <f t="shared" si="0"/>
+        <v>0.17889087656529518</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="11">
+        <v>6758</v>
+      </c>
+      <c r="C55" s="12">
+        <v>90</v>
+      </c>
+      <c r="D55" s="17">
+        <f t="shared" si="0"/>
+        <v>1.3317549570878959</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="11">
+        <v>556</v>
+      </c>
+      <c r="C56" s="12">
+        <v>0</v>
+      </c>
+      <c r="D56" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="14">
+        <v>743798</v>
+      </c>
+      <c r="C57" s="15">
+        <v>11851</v>
+      </c>
+      <c r="D57" s="19">
+        <f t="shared" si="0"/>
+        <v>1.5933089360283303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.44140625" style="6"/>
+    <col min="1" max="3" width="14.44140625" style="6"/>
+    <col min="7" max="16384" width="14.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C1" s="5"/>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -11686,17 +12583,8 @@
       <c r="C2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -11706,1170 +12594,610 @@
       <c r="C3" s="9">
         <v>28</v>
       </c>
-      <c r="D3" s="8">
-        <v>5130</v>
-      </c>
-      <c r="E3" s="9">
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="11">
+        <v>717</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="11">
+        <v>4397</v>
+      </c>
+      <c r="C5" s="12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2897</v>
+      </c>
+      <c r="C6" s="12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>39644</v>
+      </c>
+      <c r="C7" s="12">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11">
+        <v>12985</v>
+      </c>
+      <c r="C8" s="12">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="11">
+        <v>8907</v>
+      </c>
+      <c r="C9" s="12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1304</v>
+      </c>
+      <c r="C10" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2027</v>
+      </c>
+      <c r="C11" s="12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11">
+        <v>23152</v>
+      </c>
+      <c r="C12" s="12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>14977</v>
+      </c>
+      <c r="C13" s="12">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="11">
+        <v>395</v>
+      </c>
+      <c r="C14" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1046</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1416</v>
+      </c>
+      <c r="C16" s="12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="11">
+        <v>22173</v>
+      </c>
+      <c r="C17" s="12">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="11">
+        <v>6126</v>
+      </c>
+      <c r="C18" s="12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1869</v>
+      </c>
+      <c r="C19" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="11">
+        <v>1589</v>
+      </c>
+      <c r="C20" s="12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="10">
-        <f>E3/D3</f>
-        <v>5.4580896686159848E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="12">
-        <v>717</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="B21" s="11">
+        <v>2328</v>
+      </c>
+      <c r="C21" s="12">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="11">
+        <v>19653</v>
+      </c>
+      <c r="C22" s="12">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1532</v>
+      </c>
+      <c r="C23" s="12">
         <v>5</v>
       </c>
-      <c r="D4" s="12">
-        <v>717</v>
-      </c>
-      <c r="E4" s="13">
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11">
+        <v>5739</v>
+      </c>
+      <c r="C24" s="12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="11">
+        <v>22075</v>
+      </c>
+      <c r="C25" s="12">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="11">
+        <v>25093</v>
+      </c>
+      <c r="C26" s="12">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="11">
+        <v>3270</v>
+      </c>
+      <c r="C27" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="11">
+        <v>4008</v>
+      </c>
+      <c r="C28" s="12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="11">
+        <v>4132</v>
+      </c>
+      <c r="C29" s="12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="11">
+        <v>825</v>
+      </c>
+      <c r="C30" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="11">
+        <v>1447</v>
+      </c>
+      <c r="C31" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="11">
+        <v>4702</v>
+      </c>
+      <c r="C32" s="12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="11">
+        <v>1551</v>
+      </c>
+      <c r="C33" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="11">
+        <v>57202</v>
+      </c>
+      <c r="C34" s="12">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="11">
+        <v>1389</v>
+      </c>
+      <c r="C35" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="11">
+        <v>320540</v>
+      </c>
+      <c r="C36" s="12">
+        <v>3767</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="11">
+        <v>5790</v>
+      </c>
+      <c r="C37" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="11">
+        <v>553</v>
+      </c>
+      <c r="C38" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="11">
+        <v>4</v>
+      </c>
+      <c r="C39" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="11">
+        <v>7981</v>
+      </c>
+      <c r="C40" s="12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="11">
+        <v>2022</v>
+      </c>
+      <c r="C41" s="12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="11">
+        <v>3323</v>
+      </c>
+      <c r="C42" s="12">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="11">
+        <v>14707</v>
+      </c>
+      <c r="C43" s="12">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="11">
+        <v>582</v>
+      </c>
+      <c r="C44" s="12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="11">
+        <v>1674</v>
+      </c>
+      <c r="C45" s="12">
         <v>5</v>
       </c>
-      <c r="F4" s="14">
-        <f t="shared" ref="F4:F58" si="0">E4/D4</f>
-        <v>6.9735006973500697E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12">
-        <v>4397</v>
-      </c>
-      <c r="C5" s="13">
-        <v>74</v>
-      </c>
-      <c r="D5" s="12">
-        <v>4397</v>
-      </c>
-      <c r="E5" s="13">
-        <v>74</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" si="0"/>
-        <v>1.6829656584034569E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="12">
-        <v>2897</v>
-      </c>
-      <c r="C6" s="13">
-        <v>21</v>
-      </c>
-      <c r="D6" s="12">
-        <v>2897</v>
-      </c>
-      <c r="E6" s="13">
-        <v>21</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="0"/>
-        <v>7.2488781498101481E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="12">
-        <v>39644</v>
-      </c>
-      <c r="C7" s="13">
-        <v>775</v>
-      </c>
-      <c r="D7" s="12">
-        <v>39644</v>
-      </c>
-      <c r="E7" s="13">
-        <v>775</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="0"/>
-        <v>1.9548985975179095E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="12">
-        <v>12985</v>
-      </c>
-      <c r="C8" s="13">
-        <v>224</v>
-      </c>
-      <c r="D8" s="12">
-        <v>12985</v>
-      </c>
-      <c r="E8" s="13">
-        <v>224</v>
-      </c>
-      <c r="F8" s="14">
-        <f t="shared" si="0"/>
-        <v>1.7250673854447441E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="12">
-        <v>8907</v>
-      </c>
-      <c r="C9" s="13">
-        <v>178</v>
-      </c>
-      <c r="D9" s="12">
-        <v>8907</v>
-      </c>
-      <c r="E9" s="13">
-        <v>178</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="0"/>
-        <v>1.9984282025373303E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1304</v>
-      </c>
-      <c r="C10" s="13">
-        <v>14</v>
-      </c>
-      <c r="D10" s="12">
-        <v>1304</v>
-      </c>
-      <c r="E10" s="13">
-        <v>14</v>
-      </c>
-      <c r="F10" s="14">
-        <f t="shared" si="0"/>
-        <v>1.0736196319018405E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="11">
+        <v>4315</v>
+      </c>
+      <c r="C46" s="12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="11">
+        <v>504</v>
+      </c>
+      <c r="C47" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="11">
+        <v>8593</v>
+      </c>
+      <c r="C48" s="12">
         <v>33</v>
       </c>
-      <c r="B11" s="12">
-        <v>2027</v>
-      </c>
-      <c r="C11" s="13">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12">
-        <v>2027</v>
-      </c>
-      <c r="E11" s="13">
-        <v>23</v>
-      </c>
-      <c r="F11" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1346817957572768E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="12">
-        <v>23152</v>
-      </c>
-      <c r="C12" s="13">
-        <v>330</v>
-      </c>
-      <c r="D12" s="12">
-        <v>23152</v>
-      </c>
-      <c r="E12" s="13">
-        <v>330</v>
-      </c>
-      <c r="F12" s="14">
-        <f t="shared" si="0"/>
-        <v>1.4253628196268141E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="12">
-        <v>14977</v>
-      </c>
-      <c r="C13" s="13">
-        <v>470</v>
-      </c>
-      <c r="D13" s="12">
-        <v>14977</v>
-      </c>
-      <c r="E13" s="13">
-        <v>470</v>
-      </c>
-      <c r="F13" s="14">
-        <f t="shared" si="0"/>
-        <v>3.1381451559057222E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="12">
-        <v>395</v>
-      </c>
-      <c r="C14" s="13">
-        <v>8</v>
-      </c>
-      <c r="D14" s="12">
-        <v>395</v>
-      </c>
-      <c r="E14" s="13">
-        <v>8</v>
-      </c>
-      <c r="F14" s="14">
-        <f t="shared" si="0"/>
-        <v>2.0253164556962026E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="12">
-        <v>1046</v>
-      </c>
-      <c r="C15" s="13">
-        <v>0</v>
-      </c>
-      <c r="D15" s="12">
-        <v>1046</v>
-      </c>
-      <c r="E15" s="13">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="12">
-        <v>1416</v>
-      </c>
-      <c r="C16" s="13">
-        <v>18</v>
-      </c>
-      <c r="D16" s="12">
-        <v>1416</v>
-      </c>
-      <c r="E16" s="13">
-        <v>18</v>
-      </c>
-      <c r="F16" s="14">
-        <f t="shared" si="0"/>
-        <v>1.2711864406779662E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="12">
-        <v>22173</v>
-      </c>
-      <c r="C17" s="13">
-        <v>258</v>
-      </c>
-      <c r="D17" s="12">
-        <v>22173</v>
-      </c>
-      <c r="E17" s="13">
-        <v>258</v>
-      </c>
-      <c r="F17" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1635773237721553E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="12">
-        <v>6126</v>
-      </c>
-      <c r="C18" s="13">
-        <v>160</v>
-      </c>
-      <c r="D18" s="12">
-        <v>6126</v>
-      </c>
-      <c r="E18" s="13">
-        <v>160</v>
-      </c>
-      <c r="F18" s="14">
-        <f t="shared" si="0"/>
-        <v>2.6118184786157361E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="12">
-        <v>1869</v>
-      </c>
-      <c r="C19" s="13">
+    </row>
+    <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="11">
+        <v>13774</v>
+      </c>
+      <c r="C49" s="12">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="12">
-        <v>1869</v>
-      </c>
-      <c r="E19" s="13">
-        <v>13</v>
-      </c>
-      <c r="F19" s="14">
-        <f t="shared" si="0"/>
-        <v>6.9555912252541466E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="12">
-        <v>1589</v>
-      </c>
-      <c r="C20" s="13">
-        <v>41</v>
-      </c>
-      <c r="D20" s="12">
-        <v>1589</v>
-      </c>
-      <c r="E20" s="13">
-        <v>41</v>
-      </c>
-      <c r="F20" s="14">
-        <f t="shared" si="0"/>
-        <v>2.5802391441157962E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="12">
-        <v>2328</v>
-      </c>
-      <c r="C21" s="13">
-        <v>55</v>
-      </c>
-      <c r="D21" s="12">
-        <v>2328</v>
-      </c>
-      <c r="E21" s="13">
-        <v>55</v>
-      </c>
-      <c r="F21" s="14">
-        <f t="shared" si="0"/>
-        <v>2.3625429553264604E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="12">
-        <v>19653</v>
-      </c>
-      <c r="C22" s="13">
-        <v>710</v>
-      </c>
-      <c r="D22" s="12">
-        <v>19653</v>
-      </c>
-      <c r="E22" s="13">
-        <v>710</v>
-      </c>
-      <c r="F22" s="14">
-        <f t="shared" si="0"/>
-        <v>3.6126799979646872E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="12">
-        <v>1532</v>
-      </c>
-      <c r="C23" s="13">
+      <c r="B50" s="11">
+        <v>3873</v>
+      </c>
+      <c r="C50" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="11">
+        <v>1301</v>
+      </c>
+      <c r="C51" s="12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="11">
+        <v>170</v>
+      </c>
+      <c r="C52" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="11">
+        <v>4711</v>
+      </c>
+      <c r="C53" s="12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="12">
-        <v>1532</v>
-      </c>
-      <c r="E23" s="13">
-        <v>5</v>
-      </c>
-      <c r="F23" s="14">
-        <f t="shared" si="0"/>
-        <v>3.2637075718015664E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="12">
-        <v>5739</v>
-      </c>
-      <c r="C24" s="13">
-        <v>51</v>
-      </c>
-      <c r="D24" s="12">
-        <v>5739</v>
-      </c>
-      <c r="E24" s="13">
-        <v>51</v>
-      </c>
-      <c r="F24" s="14">
-        <f t="shared" si="0"/>
-        <v>8.8865656037637221E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="12">
-        <v>22075</v>
-      </c>
-      <c r="C25" s="13">
-        <v>195</v>
-      </c>
-      <c r="D25" s="12">
-        <v>22075</v>
-      </c>
-      <c r="E25" s="13">
-        <v>195</v>
-      </c>
-      <c r="F25" s="14">
-        <f t="shared" si="0"/>
-        <v>8.8335220838052092E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="12">
-        <v>25093</v>
-      </c>
-      <c r="C26" s="13">
-        <v>505</v>
-      </c>
-      <c r="D26" s="12">
-        <v>25093</v>
-      </c>
-      <c r="E26" s="13">
-        <v>505</v>
-      </c>
-      <c r="F26" s="14">
-        <f t="shared" si="0"/>
-        <v>2.012513449966126E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="12">
-        <v>3270</v>
-      </c>
-      <c r="C27" s="13">
-        <v>25</v>
-      </c>
-      <c r="D27" s="12">
-        <v>3270</v>
-      </c>
-      <c r="E27" s="13">
-        <v>25</v>
-      </c>
-      <c r="F27" s="14">
-        <f t="shared" si="0"/>
-        <v>7.6452599388379203E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="12">
-        <v>4008</v>
-      </c>
-      <c r="C28" s="13">
-        <v>52</v>
-      </c>
-      <c r="D28" s="12">
-        <v>4008</v>
-      </c>
-      <c r="E28" s="13">
-        <v>52</v>
-      </c>
-      <c r="F28" s="14">
-        <f t="shared" si="0"/>
-        <v>1.2974051896207584E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="12">
-        <v>4132</v>
-      </c>
-      <c r="C29" s="13">
-        <v>67</v>
-      </c>
-      <c r="D29" s="12">
-        <v>4132</v>
-      </c>
-      <c r="E29" s="13">
-        <v>67</v>
-      </c>
-      <c r="F29" s="14">
-        <f t="shared" si="0"/>
-        <v>1.6214908034849953E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="12">
-        <v>825</v>
-      </c>
-      <c r="C30" s="13">
-        <v>3</v>
-      </c>
-      <c r="D30" s="12">
-        <v>825</v>
-      </c>
-      <c r="E30" s="13">
-        <v>3</v>
-      </c>
-      <c r="F30" s="14">
-        <f t="shared" si="0"/>
-        <v>3.6363636363636364E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="12">
-        <v>1447</v>
-      </c>
-      <c r="C31" s="13">
-        <v>6</v>
-      </c>
-      <c r="D31" s="12">
-        <v>1447</v>
-      </c>
-      <c r="E31" s="13">
-        <v>6</v>
-      </c>
-      <c r="F31" s="14">
-        <f t="shared" si="0"/>
-        <v>4.1465100207325502E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="12">
-        <v>4702</v>
-      </c>
-      <c r="C32" s="13">
-        <v>79</v>
-      </c>
-      <c r="D32" s="12">
-        <v>4702</v>
-      </c>
-      <c r="E32" s="13">
-        <v>79</v>
-      </c>
-      <c r="F32" s="14">
-        <f t="shared" si="0"/>
-        <v>1.6801361122926413E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="12">
-        <v>1551</v>
-      </c>
-      <c r="C33" s="13">
-        <v>11</v>
-      </c>
-      <c r="D33" s="12">
-        <v>1551</v>
-      </c>
-      <c r="E33" s="13">
-        <v>11</v>
-      </c>
-      <c r="F33" s="14">
-        <f t="shared" si="0"/>
-        <v>7.0921985815602835E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="12">
-        <v>57202</v>
-      </c>
-      <c r="C34" s="13">
-        <v>698</v>
-      </c>
-      <c r="D34" s="12">
-        <v>57202</v>
-      </c>
-      <c r="E34" s="13">
-        <v>698</v>
-      </c>
-      <c r="F34" s="14">
-        <f t="shared" si="0"/>
-        <v>1.2202370546484388E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="12">
-        <v>1389</v>
-      </c>
-      <c r="C35" s="13">
-        <v>7</v>
-      </c>
-      <c r="D35" s="12">
-        <v>1389</v>
-      </c>
-      <c r="E35" s="13">
-        <v>7</v>
-      </c>
-      <c r="F35" s="14">
-        <f t="shared" si="0"/>
-        <v>5.0395968322534193E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="12">
-        <v>320540</v>
-      </c>
-      <c r="C36" s="13">
-        <v>3767</v>
-      </c>
-      <c r="D36" s="12">
-        <v>320540</v>
-      </c>
-      <c r="E36" s="13">
-        <v>3767</v>
-      </c>
-      <c r="F36" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1752043426717415E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="12">
-        <v>5790</v>
-      </c>
-      <c r="C37" s="13">
-        <v>16</v>
-      </c>
-      <c r="D37" s="12">
-        <v>5790</v>
-      </c>
-      <c r="E37" s="13">
-        <v>16</v>
-      </c>
-      <c r="F37" s="14">
-        <f t="shared" si="0"/>
-        <v>2.7633851468048358E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="12">
-        <v>553</v>
-      </c>
-      <c r="C38" s="13">
-        <v>3</v>
-      </c>
-      <c r="D38" s="12">
-        <v>553</v>
-      </c>
-      <c r="E38" s="13">
-        <v>3</v>
-      </c>
-      <c r="F38" s="14">
-        <f t="shared" si="0"/>
-        <v>5.4249547920433997E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="12">
-        <v>4</v>
-      </c>
-      <c r="C39" s="13">
-        <v>0</v>
-      </c>
-      <c r="D39" s="12">
-        <v>4</v>
-      </c>
-      <c r="E39" s="13">
-        <v>0</v>
-      </c>
-      <c r="F39" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="12">
-        <v>7981</v>
-      </c>
-      <c r="C40" s="13">
-        <v>124</v>
-      </c>
-      <c r="D40" s="12">
-        <v>7981</v>
-      </c>
-      <c r="E40" s="13">
-        <v>124</v>
-      </c>
-      <c r="F40" s="14">
-        <f t="shared" si="0"/>
-        <v>1.5536900137827339E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="12">
-        <v>2022</v>
-      </c>
-      <c r="C41" s="13">
-        <v>61</v>
-      </c>
-      <c r="D41" s="12">
-        <v>2022</v>
-      </c>
-      <c r="E41" s="13">
-        <v>61</v>
-      </c>
-      <c r="F41" s="14">
-        <f t="shared" si="0"/>
-        <v>3.0168150346191889E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="12">
-        <v>3323</v>
-      </c>
-      <c r="C42" s="13">
-        <v>95</v>
-      </c>
-      <c r="D42" s="12">
-        <v>3323</v>
-      </c>
-      <c r="E42" s="13">
-        <v>95</v>
-      </c>
-      <c r="F42" s="14">
-        <f t="shared" si="0"/>
-        <v>2.8588624736683721E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="12">
-        <v>14707</v>
-      </c>
-      <c r="C43" s="13">
-        <v>146</v>
-      </c>
-      <c r="D43" s="12">
-        <v>14707</v>
-      </c>
-      <c r="E43" s="13">
-        <v>146</v>
-      </c>
-      <c r="F43" s="14">
-        <f t="shared" si="0"/>
-        <v>9.9272455293397694E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="12">
-        <v>582</v>
-      </c>
-      <c r="C44" s="13">
-        <v>21</v>
-      </c>
-      <c r="D44" s="12">
-        <v>582</v>
-      </c>
-      <c r="E44" s="13">
-        <v>21</v>
-      </c>
-      <c r="F44" s="14">
-        <f t="shared" si="0"/>
-        <v>3.608247422680412E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="12">
-        <v>1674</v>
-      </c>
-      <c r="C45" s="13">
-        <v>5</v>
-      </c>
-      <c r="D45" s="12">
-        <v>1674</v>
-      </c>
-      <c r="E45" s="13">
-        <v>5</v>
-      </c>
-      <c r="F45" s="14">
-        <f t="shared" si="0"/>
-        <v>2.9868578255675031E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="12">
-        <v>4315</v>
-      </c>
-      <c r="C46" s="13">
-        <v>85</v>
-      </c>
-      <c r="D46" s="12">
-        <v>4315</v>
-      </c>
-      <c r="E46" s="13">
-        <v>85</v>
-      </c>
-      <c r="F46" s="14">
-        <f t="shared" si="0"/>
-        <v>1.9698725376593278E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="12">
-        <v>504</v>
-      </c>
-      <c r="C47" s="13">
-        <v>20</v>
-      </c>
-      <c r="D47" s="12">
-        <v>504</v>
-      </c>
-      <c r="E47" s="13">
-        <v>20</v>
-      </c>
-      <c r="F47" s="14">
-        <f t="shared" si="0"/>
-        <v>3.968253968253968E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="12">
-        <v>8593</v>
-      </c>
-      <c r="C48" s="13">
-        <v>33</v>
-      </c>
-      <c r="D48" s="12">
-        <v>8593</v>
-      </c>
-      <c r="E48" s="13">
-        <v>33</v>
-      </c>
-      <c r="F48" s="14">
-        <f t="shared" si="0"/>
-        <v>3.8403351565227512E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="12">
-        <v>13774</v>
-      </c>
-      <c r="C49" s="13">
-        <v>163</v>
-      </c>
-      <c r="D49" s="12">
-        <v>13774</v>
-      </c>
-      <c r="E49" s="13">
-        <v>163</v>
-      </c>
-      <c r="F49" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1833889937563525E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="12">
-        <v>3873</v>
-      </c>
-      <c r="C50" s="13">
-        <v>11</v>
-      </c>
-      <c r="D50" s="12">
-        <v>3873</v>
-      </c>
-      <c r="E50" s="13">
-        <v>11</v>
-      </c>
-      <c r="F50" s="14">
-        <f t="shared" si="0"/>
-        <v>2.8401755744900596E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="12">
-        <v>1301</v>
-      </c>
-      <c r="C51" s="13">
-        <v>68</v>
-      </c>
-      <c r="D51" s="12">
-        <v>1301</v>
-      </c>
-      <c r="E51" s="13">
-        <v>68</v>
-      </c>
-      <c r="F51" s="14">
-        <f t="shared" si="0"/>
-        <v>5.2267486548808612E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="12">
-        <v>170</v>
-      </c>
-      <c r="C52" s="13">
-        <v>0</v>
-      </c>
-      <c r="D52" s="12">
-        <v>170</v>
-      </c>
-      <c r="E52" s="13">
-        <v>0</v>
-      </c>
-      <c r="F52" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" s="12">
-        <v>4711</v>
-      </c>
-      <c r="C53" s="13">
-        <v>109</v>
-      </c>
-      <c r="D53" s="12">
-        <v>4711</v>
-      </c>
-      <c r="E53" s="13">
-        <v>109</v>
-      </c>
-      <c r="F53" s="14">
-        <f t="shared" si="0"/>
-        <v>2.3137338144767566E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="12">
+      <c r="B54" s="11">
         <v>35811</v>
       </c>
-      <c r="C54" s="13">
+      <c r="C54" s="12">
         <v>1924</v>
       </c>
-      <c r="D54" s="12">
-        <v>35811</v>
-      </c>
-      <c r="E54" s="13">
-        <v>1924</v>
-      </c>
-      <c r="F54" s="14">
-        <f t="shared" si="0"/>
-        <v>5.3726508614671473E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+    </row>
+    <row r="55" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="12">
+      <c r="B55" s="11">
         <v>559</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="12">
         <v>1</v>
       </c>
-      <c r="D55" s="12">
-        <v>559</v>
-      </c>
-      <c r="E55" s="13">
-        <v>1</v>
-      </c>
-      <c r="F55" s="14">
-        <f t="shared" si="0"/>
-        <v>1.7889087656529517E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+    </row>
+    <row r="56" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="12">
+      <c r="B56" s="11">
         <v>6758</v>
       </c>
-      <c r="C56" s="13">
+      <c r="C56" s="12">
         <v>90</v>
       </c>
-      <c r="D56" s="12">
-        <v>6758</v>
-      </c>
-      <c r="E56" s="13">
-        <v>90</v>
-      </c>
-      <c r="F56" s="14">
-        <f t="shared" si="0"/>
-        <v>1.3317549570878958E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="11">
         <v>556</v>
       </c>
-      <c r="C57" s="13">
-        <v>0</v>
-      </c>
-      <c r="D57" s="12">
-        <v>556</v>
-      </c>
-      <c r="E57" s="13">
-        <v>0</v>
-      </c>
-      <c r="F57" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="C57" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="16">
+      <c r="B58" s="14">
         <v>743798</v>
       </c>
-      <c r="C58" s="17">
+      <c r="C58" s="15">
         <v>11851</v>
-      </c>
-      <c r="D58" s="16">
-        <v>743798</v>
-      </c>
-      <c r="E58" s="17">
-        <v>11851</v>
-      </c>
-      <c r="F58" s="18">
-        <f t="shared" si="0"/>
-        <v>1.5933089360283304E-2</v>
       </c>
     </row>
   </sheetData>
@@ -12944,7 +13272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>